<commit_message>
EPBDS-8844 Remove workaround with spreadsheetResultPackage. Introduced GLOBAL table properties.
</commit_message>
<xml_diff>
--- a/Util/openl-maven-plugin/it/openl-gen-spreadsheetresults-beans/src/main/openl/rules/Main.xlsx
+++ b/Util/openl-maven-plugin/it/openl-gen-spreadsheetresults-beans/src/main/openl/rules/Main.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\OPENL\Util\openl-maven-plugin\it\openl-gen-csr-beans\src\main\openl\rules\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\OPENL\Util\openl-maven-plugin\it\openl-gen-spreadsheetresults-beans\src\main\openl\rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEB7E313-1305-423E-B163-DB6927992A24}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F3E3903-45E5-4C8B-B84E-0C4B4F750562}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15945" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -423,7 +423,7 @@
     <t>org.openl.generated.outputmodel</t>
   </si>
   <si>
-    <t>Module</t>
+    <t>Global</t>
   </si>
 </sst>
 </file>

</xml_diff>